<commit_message>
change add_data default setting to removeCellStyle = FALSE
</commit_message>
<xml_diff>
--- a/inst/extdata/oxlsx2_sheet.xlsx
+++ b/inst/extdata/oxlsx2_sheet.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CBC5D68-7757-461D-BB53-651353D255CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janmarvingarbuszus/Source/openxlsx2/inst/extdata/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E33989-6D2C-2047-8C34-843A72DA2D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUM" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="16">
   <si>
     <t>Header</t>
   </si>
@@ -74,6 +79,9 @@
   </si>
   <si>
     <t>V3_rel</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -87,7 +95,7 @@
     <numFmt numFmtId="167" formatCode="0.00\ %"/>
     <numFmt numFmtId="168" formatCode="0\ %"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -260,23 +268,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,15 +306,23 @@
     <xf numFmtId="167" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,469 +711,517 @@
   <dimension ref="B2:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A17" sqref="A17:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-    </row>
-    <row r="3" spans="2:9">
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="6" t="s">
+      <c r="F3" s="28"/>
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:9">
-      <c r="B4" s="4"/>
-      <c r="C4" s="7" t="s">
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B4" s="26"/>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:9" hidden="1">
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="2:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
-      <c r="B6" s="20">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B6" s="15">
         <v>44197</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="16">
         <v>1000000</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="23">
+      <c r="D6" s="17"/>
+      <c r="E6" s="18">
         <v>431</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="14">
+      <c r="F6" s="19"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="9">
         <v>29</v>
       </c>
-      <c r="I6" s="25"/>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="20">
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B7" s="15">
         <v>44228</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="16">
         <v>263654</v>
       </c>
-      <c r="D7" s="26">
-        <f>C7/C6</f>
+      <c r="D7" s="21">
+        <f t="shared" ref="D7:D16" si="0">C7/C6</f>
         <v>0.263654</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="18">
         <v>777</v>
       </c>
-      <c r="F7" s="24">
-        <f>E7/E6</f>
+      <c r="F7" s="19">
+        <f t="shared" ref="F7:F16" si="1">E7/E6</f>
         <v>1.802784222737819</v>
       </c>
-      <c r="G7" s="17">
-        <f>C7*1.2</f>
+      <c r="G7" s="12">
+        <f t="shared" ref="G7:G16" si="2">C7*1.2</f>
         <v>316384.8</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="9">
         <v>28</v>
       </c>
-      <c r="I7" s="25">
-        <f>H7/H6</f>
+      <c r="I7" s="20">
+        <f t="shared" ref="I7:I16" si="3">H7/H6</f>
         <v>0.96551724137931039</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="20">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B8" s="15">
         <v>44256</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="16">
         <v>3646</v>
       </c>
-      <c r="D8" s="26">
-        <f>C8/C7</f>
+      <c r="D8" s="21">
+        <f t="shared" si="0"/>
         <v>1.3828730078056847E-2</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="18">
         <v>4567</v>
       </c>
-      <c r="F8" s="24">
-        <f>E8/E7</f>
+      <c r="F8" s="19">
+        <f t="shared" si="1"/>
         <v>5.8777348777348779</v>
       </c>
-      <c r="G8" s="17">
-        <f>C8*1.2</f>
+      <c r="G8" s="12">
+        <f t="shared" si="2"/>
         <v>4375.2</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="9">
         <v>27</v>
       </c>
-      <c r="I8" s="25">
-        <f>H8/H7</f>
+      <c r="I8" s="20">
+        <f t="shared" si="3"/>
         <v>0.9642857142857143</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
-      <c r="B9" s="20">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B9" s="15">
         <v>44287</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="16">
         <v>4393123</v>
       </c>
-      <c r="D9" s="26">
-        <f>C9/C8</f>
+      <c r="D9" s="21">
+        <f t="shared" si="0"/>
         <v>1204.9157981349424</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="18">
         <v>464</v>
       </c>
-      <c r="F9" s="24">
-        <f>E9/E8</f>
+      <c r="F9" s="19">
+        <f t="shared" si="1"/>
         <v>0.10159842347273922</v>
       </c>
-      <c r="G9" s="17">
-        <f>C9*1.2</f>
+      <c r="G9" s="12">
+        <f t="shared" si="2"/>
         <v>5271747.5999999996</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="9">
         <v>26</v>
       </c>
-      <c r="I9" s="25">
-        <f>H9/H8</f>
+      <c r="I9" s="20">
+        <f t="shared" si="3"/>
         <v>0.96296296296296291</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
-      <c r="B10" s="20">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B10" s="15">
         <v>44317</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="16">
         <v>53123</v>
       </c>
-      <c r="D10" s="26">
-        <f>C10/C9</f>
+      <c r="D10" s="21">
+        <f t="shared" si="0"/>
         <v>1.2092308819944263E-2</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="18">
         <v>433</v>
       </c>
-      <c r="F10" s="24">
-        <f>E10/E9</f>
+      <c r="F10" s="19">
+        <f t="shared" si="1"/>
         <v>0.93318965517241381</v>
       </c>
-      <c r="G10" s="17">
-        <f>C10*1.2</f>
+      <c r="G10" s="12">
+        <f t="shared" si="2"/>
         <v>63747.6</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="9">
         <v>25</v>
       </c>
-      <c r="I10" s="25">
-        <f>H10/H9</f>
+      <c r="I10" s="20">
+        <f t="shared" si="3"/>
         <v>0.96153846153846156</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
-      <c r="B11" s="20">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B11" s="15">
         <v>44348</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="16">
         <v>63333</v>
       </c>
-      <c r="D11" s="26">
-        <f>C11/C10</f>
+      <c r="D11" s="21">
+        <f t="shared" si="0"/>
         <v>1.1921954708883158</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="18">
         <v>356</v>
       </c>
-      <c r="F11" s="24">
-        <f>E11/E10</f>
+      <c r="F11" s="19">
+        <f t="shared" si="1"/>
         <v>0.8221709006928406</v>
       </c>
-      <c r="G11" s="17">
-        <f>C11*1.2</f>
+      <c r="G11" s="12">
+        <f t="shared" si="2"/>
         <v>75999.599999999991</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="9">
         <v>24</v>
       </c>
-      <c r="I11" s="25">
-        <f>H11/H10</f>
+      <c r="I11" s="20">
+        <f t="shared" si="3"/>
         <v>0.96</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
-      <c r="B12" s="20">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B12" s="15">
         <v>44378</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="16">
         <v>838238</v>
       </c>
-      <c r="D12" s="26">
-        <f>C12/C11</f>
+      <c r="D12" s="21">
+        <f t="shared" si="0"/>
         <v>13.235406502139485</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="18">
         <v>354</v>
       </c>
-      <c r="F12" s="24">
-        <f>E12/E11</f>
+      <c r="F12" s="19">
+        <f t="shared" si="1"/>
         <v>0.9943820224719101</v>
       </c>
-      <c r="G12" s="17">
-        <f>C12*1.2</f>
+      <c r="G12" s="12">
+        <f t="shared" si="2"/>
         <v>1005885.6</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="9">
         <v>23</v>
       </c>
-      <c r="I12" s="25">
-        <f>H12/H11</f>
+      <c r="I12" s="20">
+        <f t="shared" si="3"/>
         <v>0.95833333333333337</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
-      <c r="B13" s="20">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B13" s="15">
         <v>44409</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="16">
         <v>23131239</v>
       </c>
-      <c r="D13" s="26">
-        <f>C13/C12</f>
+      <c r="D13" s="21">
+        <f t="shared" si="0"/>
         <v>27.595073236956569</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="18">
         <v>3355</v>
       </c>
-      <c r="F13" s="24">
-        <f>E13/E12</f>
+      <c r="F13" s="19">
+        <f t="shared" si="1"/>
         <v>9.4774011299435035</v>
       </c>
-      <c r="G13" s="17">
-        <f>C13*1.2</f>
+      <c r="G13" s="12">
+        <f t="shared" si="2"/>
         <v>27757486.800000001</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="9">
         <v>22</v>
       </c>
-      <c r="I13" s="25">
-        <f>H13/H12</f>
+      <c r="I13" s="20">
+        <f t="shared" si="3"/>
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
-      <c r="B14" s="20">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B14" s="15">
         <v>44440</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="16">
         <v>2323123</v>
       </c>
-      <c r="D14" s="26">
-        <f>C14/C13</f>
+      <c r="D14" s="21">
+        <f t="shared" si="0"/>
         <v>0.10043227688754588</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="18">
         <v>334</v>
       </c>
-      <c r="F14" s="24">
-        <f>E14/E13</f>
+      <c r="F14" s="19">
+        <f t="shared" si="1"/>
         <v>9.9552906110283154E-2</v>
       </c>
-      <c r="G14" s="17">
-        <f>C14*1.2</f>
+      <c r="G14" s="12">
+        <f t="shared" si="2"/>
         <v>2787747.6</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="9">
         <v>21</v>
       </c>
-      <c r="I14" s="25">
-        <f>H14/H13</f>
+      <c r="I14" s="20">
+        <f t="shared" si="3"/>
         <v>0.95454545454545459</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
-      <c r="B15" s="20">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B15" s="15">
         <v>44470</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="16">
         <v>3323123</v>
       </c>
-      <c r="D15" s="26">
-        <f>C15/C14</f>
+      <c r="D15" s="21">
+        <f t="shared" si="0"/>
         <v>1.4304550383255643</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="18">
         <v>541</v>
       </c>
-      <c r="F15" s="24">
-        <f>E15/E14</f>
+      <c r="F15" s="19">
+        <f t="shared" si="1"/>
         <v>1.6197604790419162</v>
       </c>
-      <c r="G15" s="17">
-        <f>C15*1.2</f>
+      <c r="G15" s="12">
+        <f t="shared" si="2"/>
         <v>3987747.5999999996</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="9">
         <v>20</v>
       </c>
-      <c r="I15" s="25">
-        <f>H15/H14</f>
+      <c r="I15" s="20">
+        <f t="shared" si="3"/>
         <v>0.95238095238095233</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
-      <c r="B16" s="20">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B16" s="15">
         <v>44501</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="16">
         <v>35344</v>
       </c>
-      <c r="D16" s="26">
-        <f>C16/C15</f>
+      <c r="D16" s="21">
+        <f t="shared" si="0"/>
         <v>1.0635778452979321E-2</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="18">
         <v>555</v>
       </c>
-      <c r="F16" s="24">
-        <f>E16/E15</f>
+      <c r="F16" s="19">
+        <f t="shared" si="1"/>
         <v>1.0258780036968578</v>
       </c>
-      <c r="G16" s="17">
-        <f>C16*1.2</f>
+      <c r="G16" s="12">
+        <f t="shared" si="2"/>
         <v>42412.799999999996</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="9">
         <v>20</v>
       </c>
-      <c r="I16" s="25">
-        <f>H16/H15</f>
+      <c r="I16" s="20">
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" hidden="1">
-      <c r="B17" s="27">
+    <row r="17" spans="2:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="22">
         <v>44531</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="19"/>
-    </row>
-    <row r="18" spans="2:9" hidden="1">
-      <c r="B18" s="27">
+      <c r="C17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="12"/>
+      <c r="H17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="22">
         <v>44562</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="19"/>
-    </row>
-    <row r="19" spans="2:9" hidden="1">
-      <c r="B19" s="27">
+      <c r="C18" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="12"/>
+      <c r="H18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="22">
         <v>44593</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="19"/>
-    </row>
-    <row r="20" spans="2:9" hidden="1">
-      <c r="B20" s="29">
+      <c r="C19" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="H19" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" hidden="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="23">
         <v>44594</v>
       </c>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
+      <c r="C20" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="24"/>
+      <c r="H20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="20" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>